<commit_message>
Added ML 4 and 5
</commit_message>
<xml_diff>
--- a/Control Frameworks/CMMC v1.02/CMMC v1.02 (All Maturity Levels).xlsx
+++ b/Control Frameworks/CMMC v1.02/CMMC v1.02 (All Maturity Levels).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsokol/Documents/git/simplerisk/import-content/Control Frameworks/CMMC v1.02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF014AC-A60D-4C4A-B9E3-45B601D318ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE72C90-D8E0-D540-B251-0CDDB3E5BE0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="460" windowWidth="30340" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20260" yWindow="460" windowWidth="30340" windowHeight="16940" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CMMC v1.02 Maturity Level 1" sheetId="3" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="CMMC v1.02 Maturity Level 4" sheetId="4" r:id="rId4"/>
     <sheet name="CMMC v1.02 Maturity Level 5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="657">
   <si>
     <t>Framework Name</t>
   </si>
@@ -2078,6 +2078,410 @@
 • NIST CSF v1.1 DE.CM-4
 • CERT RMM v1.2 VAR:SG3.SP1
 • NIST SP 800-53 Rev 4 SI-3</t>
+  </si>
+  <si>
+    <t>C006: Manage asset inventory</t>
+  </si>
+  <si>
+    <t>C033: Manage supply chain risk</t>
+  </si>
+  <si>
+    <t>AC.4.023</t>
+  </si>
+  <si>
+    <t>AC.4.025</t>
+  </si>
+  <si>
+    <t>AC.4.032</t>
+  </si>
+  <si>
+    <t>AM.4.226</t>
+  </si>
+  <si>
+    <t>AU.4.053</t>
+  </si>
+  <si>
+    <t>AU.4.054</t>
+  </si>
+  <si>
+    <t>AT.4.059</t>
+  </si>
+  <si>
+    <t>AT.4.060</t>
+  </si>
+  <si>
+    <t>CM.4.073</t>
+  </si>
+  <si>
+    <t>IR.4.100</t>
+  </si>
+  <si>
+    <t>IR.4.101</t>
+  </si>
+  <si>
+    <t>RM.4.149</t>
+  </si>
+  <si>
+    <t>RM.4.150</t>
+  </si>
+  <si>
+    <t>RM.4.151</t>
+  </si>
+  <si>
+    <t>RM.4.148</t>
+  </si>
+  <si>
+    <t>CA.4.163</t>
+  </si>
+  <si>
+    <t>CA.4.164</t>
+  </si>
+  <si>
+    <t>CA.4.227</t>
+  </si>
+  <si>
+    <t>SA.4.171</t>
+  </si>
+  <si>
+    <t>SA.4.173</t>
+  </si>
+  <si>
+    <t>SC.5.198</t>
+  </si>
+  <si>
+    <t>SC.5.230</t>
+  </si>
+  <si>
+    <t>SC.4.199</t>
+  </si>
+  <si>
+    <t>SC.4.202</t>
+  </si>
+  <si>
+    <t>SC.4.229</t>
+  </si>
+  <si>
+    <t>SI.4.221</t>
+  </si>
+  <si>
+    <t>Control information flows between security domains on connected systems.</t>
+  </si>
+  <si>
+    <t>• CMMC modification of Draft NIST SP 800-171B 3.1.3e 
+• CIS Controls v7.1 12.1, 12.2, 13.1, 13.3, 14.1, 14.2, 14.5, 14.6, 14.7, 15.6, 15.10
+• NIST CSF v1.1 ID.AM-3, PR.AC-5, PR.DS-5, PR.PT-4, DE.AE-1
+• NIST SP 800-53 Rev 4 AC-4, AC-4(1), AC-4(6), AC-4(8), AC-4(12), AC-4(13), AC-4(15), AC-4(20)</t>
+  </si>
+  <si>
+    <t>Periodically review and update CUI program access permissions.</t>
+  </si>
+  <si>
+    <t>Restrict remote network access based on organizationally defined risk factors such as time of day, location of access, physical location, network connection state, and measured properties of the current user and role.</t>
+  </si>
+  <si>
+    <t>Employ a capability to discover and identify systems with specific component attributes (e.g., firmware level, OS type) within your inventory.</t>
+  </si>
+  <si>
+    <t>• CMMC modification of Draft NIST SP 800-171B 3.4.3e
+• CIS Controls v7.1 1.1, 1.2, 1.4, 1.5, 2.3, 2.4, 2.5
+• NIST CSF v1.1 ID.AM-1, ID.AM-2
+• CERT RMM v1.2 ADM:SG1.SP1
+• NIST SP 800-53 Rev 4 CM-8</t>
+  </si>
+  <si>
+    <t>Automate analysis of audit logs to identify and act on critical indicators (TTPs) and/or organizationally defined suspicious activity.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• CMMC
+• CIS Controls v7.1 6.6
+• NIST CSF v1.1 DE.AE-3
+• NIST SP 800-53 Rev 4 SI-4(2) </t>
+  </si>
+  <si>
+    <t>Review audit information for broad activity in addition to per-machine activity.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• NIST CSF v1.1 PR.PT-1
+• NIST SP 800-53 Rev 4 RA-5(6), RA-5(8), RA-5(10)</t>
+  </si>
+  <si>
+    <t>Provide awareness training focused on recognizing and responding to threats from social engineering, advanced persistent threat actors, breaches, and suspicious behaviors; update the training at least annually or when there are significant changes to the threat.</t>
+  </si>
+  <si>
+    <t>• Draft NIST SP 800-171B 3.2.1e
+• CIS Controls v7.1 17.1, 17.2, 17.4
+• NIST CSF v1.1 PR.AT-1, PR.AT-2, PR.AT-3, PR.AT-4, PR.AT-5
+• CERT RMM v1.2 OTA:SG2.SP1
+• NIST SP 800-53 Rev 4 AT-2</t>
+  </si>
+  <si>
+    <t>Include practical exercises in awareness training that are aligned with current threat scenarios and provide feedback to individuals involved in the training.</t>
+  </si>
+  <si>
+    <t>• CMMC modification of Draft NIST SP 800-171B 3.2.2e
+• CIS Controls v7.1 17.1, 17.2, 17.4
+• NIST CSF v1.1 PR.AT-1, PR.AT-2, PR.AT-3, PR.AT-4, PR.AT-5
+• CERT RMM v1.2 OTA:SG3.SP1, OTA:SG3.SP2
+• NIST SP 800-53 Rev 4 AT-2(1)</t>
+  </si>
+  <si>
+    <t>Employ application whitelisting and an application vetting process for systems identified by the organization.</t>
+  </si>
+  <si>
+    <t>• CMMC modification of NIST SP 800-171 3.4.8
+• CIS Controls v7.1 2.1, 2.2, 2.6, 2.7, 2.8, 2.9
+• NIST CSF v1.1 PR.PT-3
+• CERT RMM v1.2 TM:SG2.SP2
+• NIST SP 800-53 Rev 4 CM-7(4), CM-7(5)</t>
+  </si>
+  <si>
+    <t>Use knowledge of attacker tactics, techniques, and procedures in incident response planning and execution.</t>
+  </si>
+  <si>
+    <t>Establish and maintain a security operations center capability that facilitates a 24/7 response capability.</t>
+  </si>
+  <si>
+    <t>• CMMC modification of Draft NIST SP 800-171B 3.6.1e</t>
+  </si>
+  <si>
+    <t>Catalog and periodically update threat profiles and adversary TTPs.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• NIST CSF v1.1 DE.AE-2
+• CERT RMM v1.2 VAR:SG2.SP1</t>
+  </si>
+  <si>
+    <t>Employ threat intelligence to inform the development of the system and security architectures, selection of security solutions, monitoring, threat hunting, and response and recovery activities.</t>
+  </si>
+  <si>
+    <t>• Draft NIST SP 800-171B 3.11.1e
+• NIST CSF v1.1 ID.RA-2, ID.RA-3</t>
+  </si>
+  <si>
+    <t>Perform scans for unauthorized ports available across perimeter network boundaries over the organization's Internet network boundaries and other organizationally defined boundaries.</t>
+  </si>
+  <si>
+    <t>• CIS Controls v7.1 12.2
+• NIST CSF v1.1 DE.CM-7</t>
+  </si>
+  <si>
+    <t>Develop and update as required, a plan for managing supply chain risks associated with the IT supply chain.</t>
+  </si>
+  <si>
+    <t>• CMMC modification of Draft NIST SP 800-171B 3.11.7e
+• NIST CSF v1.1 ID.SC-1, ID.SC-2
+• CERT RMM v1.2 EC:SG3.SP1, EC:SG3.SP2
+• NIST SP 800-53 Rev 4 SA-12</t>
+  </si>
+  <si>
+    <t>Create, maintain, and leverage a security strategy and roadmap for organizational cybersecurity improvement.</t>
+  </si>
+  <si>
+    <t>• NIST CSF v1.1 ID.RM-1, RS.IM-1, RS.IM-2, RC.IM-1, and RC.IM-2
+• NIST SP 800-53 Rev 4 PL-1</t>
+  </si>
+  <si>
+    <t>Conduct penetration testing periodically, leveraging automated scanning tools and ad hoc tests using human experts.</t>
+  </si>
+  <si>
+    <t>• CMMC modification of Draft NIST SP 800-171B 3.12.1e
+• CIS Controls v7.1 20.2
+• NIST SP 800-53 Rev 4 CA-8</t>
+  </si>
+  <si>
+    <t>Periodically perform red teaming against organizational assets in order to validate defensive capabilities.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• CIS Controls v7.1 20.3
+• NIST SP 800-53 Rev 4 CA-8(2)</t>
+  </si>
+  <si>
+    <t>Establish and maintain a cyber threat hunting capability to search for indicators of compromise in organizational systems and detect, track, and disrupt threats that evade existing controls.</t>
+  </si>
+  <si>
+    <t>• Draft NIST SP 800-171B 3.11.2e
+• NIST CSF v1.1 DE.CM-1, DE.CM-2, DE.CM-3, DE.CM-4, DE.CM-5, DE.CM-6, DE.CM.7, DE.CM-8
+• NIST SP 800-53 Rev 4 PM-16</t>
+  </si>
+  <si>
+    <t>Design network and system security capabilities to leverage, integrate, and share indicators of compromise.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• NIST SP 800-53 Rev 4 SI-4(24)</t>
+  </si>
+  <si>
+    <t>Configure monitoring systems to record packets passing through the organization's Internet network boundaries and other organizationally defined boundaries.</t>
+  </si>
+  <si>
+    <t>• CIS Controls v7.1 12.5</t>
+  </si>
+  <si>
+    <t>Enforce port and protocol compliance.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• CIS Controls v7.1 9.2
+• NIST 800-53 Rev 4 SC-7(17)</t>
+  </si>
+  <si>
+    <t>Utilize threat intelligence to proactively block DNS requests from reaching malicious domains.</t>
+  </si>
+  <si>
+    <t>Employ mechanisms to analyze executable code and scripts (e.g., sandbox) traversing Internet network boundaries or other organizationally defined boundaries.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• NIST SP 800-53 Rev 4 SC-44</t>
+  </si>
+  <si>
+    <t>Utilize a URL categorization service and implement techniques to enforce URL filtering of websites that are not approved by the organization.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• CIS Controls v7.1 7.4</t>
+  </si>
+  <si>
+    <t>Use threat indicator information relevant to the information and systems being protected and effective mitigations obtained from external organizations to inform intrusion detection and threat hunting.</t>
+  </si>
+  <si>
+    <t>• Draft NIST SP 800-171B 3.14.6e
+• NIST CSF v1.1 ID.RA-2, ID.RA-3</t>
+  </si>
+  <si>
+    <t>C030: Manage information security continuity</t>
+  </si>
+  <si>
+    <t>AC.5.024</t>
+  </si>
+  <si>
+    <t>AU.5.055</t>
+  </si>
+  <si>
+    <t>CM.5.074</t>
+  </si>
+  <si>
+    <t>IR.5.106</t>
+  </si>
+  <si>
+    <t>IR.5.102</t>
+  </si>
+  <si>
+    <t>IR.5.108</t>
+  </si>
+  <si>
+    <t>IR.5.110</t>
+  </si>
+  <si>
+    <t>RE.5.140</t>
+  </si>
+  <si>
+    <t>RM.5.152</t>
+  </si>
+  <si>
+    <t>RM.5.155</t>
+  </si>
+  <si>
+    <t>SC.5.208</t>
+  </si>
+  <si>
+    <t>SI.5.222</t>
+  </si>
+  <si>
+    <t>SI.5.223</t>
+  </si>
+  <si>
+    <t>Identify and mitigate risk associated with unidentified wireless access points connected to the network.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• CIS Controls v7.1 15.3
+• NIST CSF v1.1 PR.DS-5, DE.AE-1, DE.CM-7
+• NIST SP 800-53 Rev 4 SI-4(14)</t>
+  </si>
+  <si>
+    <t>Identify assets not reporting audit logs and assure appropriate organizationally defined systems are logging.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• CIS Controls v7.1 6.2
+• NIST SP 800-53 Rev 4 AU-12</t>
+  </si>
+  <si>
+    <t>Verify the integrity and correctness of security critical or essential software as defined by the organization (e.g., roots of trust, formal verification, or cryptographic signatures).</t>
+  </si>
+  <si>
+    <t>• CMMC modification of Draft NIST SP 800-171B 3.14.1e
+• CIS Controls v7.1 2.10
+• NIST CSF v1.1 PR.DS-6, PR.DS-8, PR.IP-2
+• CERT RMM v1.2 TM:SG2.SP2
+• NIST SP 800-53 Rev 4  SI-7(6), SI-7(9), SI-7(10), SA-17</t>
+  </si>
+  <si>
+    <t>In response to cyber incidents, utilize forensic data gathering across impacted systems, ensuring the secure transfer and protection of forensic data.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• NIST CSF v1.1 RS.AM-3
+• NIST SP 800-53 Rev 4 AU-12</t>
+  </si>
+  <si>
+    <t>Use a combination of manual and automated, real-time responses to anomalous activities that match incident patterns.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• NIST SP 800-53 Rev 4 IR-4(1)</t>
+  </si>
+  <si>
+    <t>Establish and maintain a cyber incident response team that can investigate an issue physically or virtually at any location within 24 hours.</t>
+  </si>
+  <si>
+    <t>• CMMC modification of Draft NIST SP 800-171B 3.6.2e</t>
+  </si>
+  <si>
+    <t>Perform unannounced operational exercises to demonstrate technical and procedural responses.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• CIS Controls v7.1 19.7</t>
+  </si>
+  <si>
+    <t>Ensure information processing facilities meet organizationally defined information security continuity, redundancy, and availability requirements.</t>
+  </si>
+  <si>
+    <t>• CMMC
+• NIST CSF v1.1 PR.IP-9
+• CERT RMM v1.2 RRM:SG1.SP2
+• NIST 800-53 Rev 4 CP-10</t>
+  </si>
+  <si>
+    <t>Utilize an exception process for non-whitelisted software that includes mitigation techniques.</t>
+  </si>
+  <si>
+    <t>Analyze the effectiveness of security solutions at least annually to address anticipated risk to the system and the organization based on current and accumulated threat intelligence.</t>
+  </si>
+  <si>
+    <t>• CMMC modification of Draft NIST SP 800-171B 3.11.5e
+• CERT RMM v1.2 RISK:SG6.SP1</t>
+  </si>
+  <si>
+    <t>Employ organizationally defined and tailored boundary protections in addition to commercially available solutions.</t>
+  </si>
+  <si>
+    <t>Analyze system behavior to detect and mitigate execution of normal system commands and scripts that indicate malicious actions.</t>
+  </si>
+  <si>
+    <t>Monitor individuals and system components on an ongoing basis for anomalous or suspicious behavior.</t>
+  </si>
+  <si>
+    <t>• Draft NIST SP 800-171B 3.14.2e
+• CIS Controls v7.1 13.3, 16.12, 16.13
+• NIST CSF v1.1 DE.CM-1, DE.CM-3
+• CERT RMM v1.2 MON:SG1.SP3
+• NIST SP 800-53 Rev 4 SI-4</t>
   </si>
 </sst>
 </file>
@@ -2581,10 +2985,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -2942,7 +3346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1181B36C-6D61-4E43-8411-924D05A97DEE}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -2957,470 +3361,470 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>502</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="2" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="2" t="s">
         <v>543</v>
       </c>
     </row>
@@ -6413,7 +6817,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:C76"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -8798,20 +9204,1481 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95FA5B7-9436-324E-80C2-1BF95F9E19C1}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="230.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="221.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="245.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="str">
+        <f>"CMMC v1.02 Maturity Level 4"</f>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>_xlfn.CONCAT("MC01: Improve ",I2," activities")</f>
+        <v>MC01: Improve Access Control activities</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>_xlfn.CONCAT(J2,".4.996")</f>
+        <v>AC.4.996</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>D2</f>
+        <v>AC.4.996</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>_xlfn.CONCAT(D2,": ", G2)</f>
+        <v>AC.4.996: Review and measure Access Control activities for effectiveness.</v>
+      </c>
+      <c r="G2" s="1" t="str">
+        <f>_xlfn.CONCAT("Review and measure ",I2," activities for effectiveness.")</f>
+        <v>Review and measure Access Control activities for effectiveness.</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="str">
+        <f t="shared" ref="A3:A44" si="0">"CMMC v1.02 Maturity Level 4"</f>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f t="shared" ref="C3:C18" si="1">_xlfn.CONCAT("MC01: Improve ",I3," activities")</f>
+        <v>MC01: Improve Asset Management activities</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f t="shared" ref="D3:D18" si="2">_xlfn.CONCAT(J3,".4.996")</f>
+        <v>AM.4.996</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f t="shared" ref="E3:E44" si="3">D3</f>
+        <v>AM.4.996</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f t="shared" ref="F3:F44" si="4">_xlfn.CONCAT(D3,": ", G3)</f>
+        <v>AM.4.996: Review and measure Asset Management activities for effectiveness.</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <f t="shared" ref="G3:G18" si="5">_xlfn.CONCAT("Review and measure ",I3," activities for effectiveness.")</f>
+        <v>Review and measure Asset Management activities for effectiveness.</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Audit and Accountability activities</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AU.4.996</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AU.4.996</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AU.4.996: Review and measure Audit and Accountability activities for effectiveness.</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Audit and Accountability activities for effectiveness.</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Awareness and Training activities</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>AT.4.996</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AT.4.996</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AT.4.996: Review and measure Awareness and Training activities for effectiveness.</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Awareness and Training activities for effectiveness.</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Configuration Management activities</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>CM.4.996</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CM.4.996</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>CM.4.996: Review and measure Configuration Management activities for effectiveness.</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Configuration Management activities for effectiveness.</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Identification and Authentication activities</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>IA.4.996</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>IA.4.996</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>IA.4.996: Review and measure Identification and Authentication activities for effectiveness.</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Identification and Authentication activities for effectiveness.</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Incident Response activities</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>IR.4.996</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>IR.4.996</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>IR.4.996: Review and measure Incident Response activities for effectiveness.</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Incident Response activities for effectiveness.</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Maintenance activities</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>MA.4.996</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>MA.4.996</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>MA.4.996: Review and measure Maintenance activities for effectiveness.</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Maintenance activities for effectiveness.</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Media Protection activities</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>MP.4.996</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>MP.4.996</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>MP.4.996: Review and measure Media Protection activities for effectiveness.</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Media Protection activities for effectiveness.</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Personnel Security activities</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>PS.4.996</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>PS.4.996</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>PS.4.996: Review and measure Personnel Security activities for effectiveness.</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Personnel Security activities for effectiveness.</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Physical Protection activities</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>PE.4.996</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>PE.4.996</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>PE.4.996: Review and measure Physical Protection activities for effectiveness.</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Physical Protection activities for effectiveness.</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Recovery activities</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>RE.4.996</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>RE.4.996</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>RE.4.996: Review and measure Recovery activities for effectiveness.</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Recovery activities for effectiveness.</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Risk Management activities</v>
+      </c>
+      <c r="D14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>RM.4.996</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>RM.4.996</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>RM.4.996: Review and measure Risk Management activities for effectiveness.</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Risk Management activities for effectiveness.</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Security Assessment activities</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>CA.4.996</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CA.4.996</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>CA.4.996: Review and measure Security Assessment activities for effectiveness.</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Security Assessment activities for effectiveness.</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve Situational Awareness activities</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>SA.4.996</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SA.4.996</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>SA.4.996: Review and measure Situational Awareness activities for effectiveness.</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure Situational Awareness activities for effectiveness.</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve System and Communications Protection activities</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>SC.4.996</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SC.4.996</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>SC.4.996: Review and measure System and Communications Protection activities for effectiveness.</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure System and Communications Protection activities for effectiveness.</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>MC01: Improve System and Information Integrity activities</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>SI.4.996</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SI.4.996</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>SI.4.996: Review and measure System and Information Integrity activities for effectiveness.</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>Review and measure System and Information Integrity activities for effectiveness.</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="E19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AC.4.023</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AC.4.023: Control information flows between security domains on connected systems.</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AC.4.025</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AC.4.025: Periodically review and update CUI program access permissions.</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="E21" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AC.4.032</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AC.4.032: Restrict remote network access based on organizationally defined risk factors such as time of day, location of access, physical location, network connection state, and measured properties of the current user and role.</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="E22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AM.4.226</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AM.4.226: Employ a capability to discover and identify systems with specific component attributes (e.g., firmware level, OS type) within your inventory.</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="E23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AU.4.053</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AU.4.053: Automate analysis of audit logs to identify and act on critical indicators (TTPs) and/or organizationally defined suspicious activity.</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="E24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AU.4.054</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AU.4.054: Review audit information for broad activity in addition to per-machine activity.</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="E25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AT.4.059</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AT.4.059: Provide awareness training focused on recognizing and responding to threats from social engineering, advanced persistent threat actors, breaches, and suspicious behaviors; update the training at least annually or when there are significant changes to the threat.</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AT.4.060</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>AT.4.060: Include practical exercises in awareness training that are aligned with current threat scenarios and provide feedback to individuals involved in the training.</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CM.4.073</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>CM.4.073: Employ application whitelisting and an application vetting process for systems identified by the organization.</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="E28" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>IR.4.100</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>IR.4.100: Use knowledge of attacker tactics, techniques, and procedures in incident response planning and execution.</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="E29" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>IR.4.101</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>IR.4.101: Establish and maintain a security operations center capability that facilitates a 24/7 response capability.</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>RM.4.149</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>RM.4.149: Catalog and periodically update threat profiles and adversary TTPs.</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="E31" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>RM.4.150</v>
+      </c>
+      <c r="F31" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>RM.4.150: Employ threat intelligence to inform the development of the system and security architectures, selection of security solutions, monitoring, threat hunting, and response and recovery activities.</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="E32" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>RM.4.151</v>
+      </c>
+      <c r="F32" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>RM.4.151: Perform scans for unauthorized ports available across perimeter network boundaries over the organization's Internet network boundaries and other organizationally defined boundaries.</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="E33" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>RM.4.148</v>
+      </c>
+      <c r="F33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>RM.4.148: Develop and update as required, a plan for managing supply chain risks associated with the IT supply chain.</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="E34" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CA.4.163</v>
+      </c>
+      <c r="F34" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>CA.4.163: Create, maintain, and leverage a security strategy and roadmap for organizational cybersecurity improvement.</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="E35" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CA.4.164</v>
+      </c>
+      <c r="F35" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>CA.4.164: Conduct penetration testing periodically, leveraging automated scanning tools and ad hoc tests using human experts.</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="E36" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CA.4.227</v>
+      </c>
+      <c r="F36" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>CA.4.227: Periodically perform red teaming against organizational assets in order to validate defensive capabilities.</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E37" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SA.4.171</v>
+      </c>
+      <c r="F37" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>SA.4.171: Establish and maintain a cyber threat hunting capability to search for indicators of compromise in organizational systems and detect, track, and disrupt threats that evade existing controls.</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="E38" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SA.4.173</v>
+      </c>
+      <c r="F38" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>SA.4.173: Design network and system security capabilities to leverage, integrate, and share indicators of compromise.</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="E39" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SC.5.198</v>
+      </c>
+      <c r="F39" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>SC.5.198: Configure monitoring systems to record packets passing through the organization's Internet network boundaries and other organizationally defined boundaries.</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="E40" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SC.5.230</v>
+      </c>
+      <c r="F40" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>SC.5.230: Enforce port and protocol compliance.</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="E41" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SC.4.199</v>
+      </c>
+      <c r="F41" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>SC.4.199: Utilize threat intelligence to proactively block DNS requests from reaching malicious domains.</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="E42" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SC.4.202</v>
+      </c>
+      <c r="F42" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>SC.4.202: Employ mechanisms to analyze executable code and scripts (e.g., sandbox) traversing Internet network boundaries or other organizationally defined boundaries.</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="E43" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SC.4.229</v>
+      </c>
+      <c r="F43" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>SC.4.229: Utilize a URL categorization service and implement techniques to enforce URL filtering of websites that are not approved by the organization.</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 4</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="E44" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SI.4.221</v>
+      </c>
+      <c r="F44" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>SI.4.221: Use threat indicator information relevant to the information and systems being protected and effective mitigations obtained from external organizations to inform intrusion detection and threat hunting.</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E78D9C1-42B5-894D-AC78-ACB22999BE15}">
+  <dimension ref="A1:J33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="88.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="80.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="70.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="162.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="153" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="175" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -8848,710 +10715,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17">
-      <c r="A2" s="1" t="str">
-        <f>"CMMC v1.02 Maturity Level 4"</f>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <f>_xlfn.CONCAT("MC01: Improve ",I2," activities")</f>
-        <v>MC01: Improve Access Control activities</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <f>_xlfn.CONCAT(J2,".4.996")</f>
-        <v>AC.4.996</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <f>D2</f>
-        <v>AC.4.996</v>
-      </c>
-      <c r="F2" s="1" t="str">
-        <f>_xlfn.CONCAT(D2,": ", G2)</f>
-        <v>AC.4.996: Review and measure Access Control activities for effectiveness.</v>
-      </c>
-      <c r="G2" s="2" t="str">
-        <f>_xlfn.CONCAT("Review and measure ",I2," activities for effectiveness.")</f>
-        <v>Review and measure Access Control activities for effectiveness.</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="17">
-      <c r="A3" s="1" t="str">
-        <f t="shared" ref="A3:A18" si="0">"CMMC v1.02 Maturity Level 4"</f>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="str">
-        <f t="shared" ref="C3:C18" si="1">_xlfn.CONCAT("MC01: Improve ",I3," activities")</f>
-        <v>MC01: Improve Asset Management activities</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D18" si="2">_xlfn.CONCAT(J3,".4.996")</f>
-        <v>AM.4.996</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <f t="shared" ref="E3:E18" si="3">D3</f>
-        <v>AM.4.996</v>
-      </c>
-      <c r="F3" s="1" t="str">
-        <f t="shared" ref="F3:F18" si="4">_xlfn.CONCAT(D3,": ", G3)</f>
-        <v>AM.4.996: Review and measure Asset Management activities for effectiveness.</v>
-      </c>
-      <c r="G3" s="2" t="str">
-        <f t="shared" ref="G3:G18" si="5">_xlfn.CONCAT("Review and measure ",I3," activities for effectiveness.")</f>
-        <v>Review and measure Asset Management activities for effectiveness.</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="17">
-      <c r="A4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Audit and Accountability activities</v>
-      </c>
-      <c r="D4" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>AU.4.996</v>
-      </c>
-      <c r="E4" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>AU.4.996</v>
-      </c>
-      <c r="F4" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>AU.4.996: Review and measure Audit and Accountability activities for effectiveness.</v>
-      </c>
-      <c r="G4" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Audit and Accountability activities for effectiveness.</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17">
-      <c r="A5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Awareness and Training activities</v>
-      </c>
-      <c r="D5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>AT.4.996</v>
-      </c>
-      <c r="E5" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>AT.4.996</v>
-      </c>
-      <c r="F5" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>AT.4.996: Review and measure Awareness and Training activities for effectiveness.</v>
-      </c>
-      <c r="G5" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Awareness and Training activities for effectiveness.</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="17">
-      <c r="A6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Configuration Management activities</v>
-      </c>
-      <c r="D6" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CM.4.996</v>
-      </c>
-      <c r="E6" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>CM.4.996</v>
-      </c>
-      <c r="F6" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>CM.4.996: Review and measure Configuration Management activities for effectiveness.</v>
-      </c>
-      <c r="G6" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Configuration Management activities for effectiveness.</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="17">
-      <c r="A7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Identification and Authentication activities</v>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>IA.4.996</v>
-      </c>
-      <c r="E7" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>IA.4.996</v>
-      </c>
-      <c r="F7" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>IA.4.996: Review and measure Identification and Authentication activities for effectiveness.</v>
-      </c>
-      <c r="G7" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Identification and Authentication activities for effectiveness.</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="17">
-      <c r="A8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Incident Response activities</v>
-      </c>
-      <c r="D8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>IR.4.996</v>
-      </c>
-      <c r="E8" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>IR.4.996</v>
-      </c>
-      <c r="F8" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>IR.4.996: Review and measure Incident Response activities for effectiveness.</v>
-      </c>
-      <c r="G8" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Incident Response activities for effectiveness.</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="17">
-      <c r="A9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Maintenance activities</v>
-      </c>
-      <c r="D9" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>MA.4.996</v>
-      </c>
-      <c r="E9" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>MA.4.996</v>
-      </c>
-      <c r="F9" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>MA.4.996: Review and measure Maintenance activities for effectiveness.</v>
-      </c>
-      <c r="G9" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Maintenance activities for effectiveness.</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="17">
-      <c r="A10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Media Protection activities</v>
-      </c>
-      <c r="D10" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>MP.4.996</v>
-      </c>
-      <c r="E10" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>MP.4.996</v>
-      </c>
-      <c r="F10" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>MP.4.996: Review and measure Media Protection activities for effectiveness.</v>
-      </c>
-      <c r="G10" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Media Protection activities for effectiveness.</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17">
-      <c r="A11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Personnel Security activities</v>
-      </c>
-      <c r="D11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>PS.4.996</v>
-      </c>
-      <c r="E11" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>PS.4.996</v>
-      </c>
-      <c r="F11" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>PS.4.996: Review and measure Personnel Security activities for effectiveness.</v>
-      </c>
-      <c r="G11" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Personnel Security activities for effectiveness.</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="17">
-      <c r="A12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Physical Protection activities</v>
-      </c>
-      <c r="D12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>PE.4.996</v>
-      </c>
-      <c r="E12" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>PE.4.996</v>
-      </c>
-      <c r="F12" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>PE.4.996: Review and measure Physical Protection activities for effectiveness.</v>
-      </c>
-      <c r="G12" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Physical Protection activities for effectiveness.</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17">
-      <c r="A13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Recovery activities</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>RE.4.996</v>
-      </c>
-      <c r="E13" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>RE.4.996</v>
-      </c>
-      <c r="F13" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>RE.4.996: Review and measure Recovery activities for effectiveness.</v>
-      </c>
-      <c r="G13" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Recovery activities for effectiveness.</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="17">
-      <c r="A14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Risk Management activities</v>
-      </c>
-      <c r="D14" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>RM.4.996</v>
-      </c>
-      <c r="E14" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>RM.4.996</v>
-      </c>
-      <c r="F14" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>RM.4.996: Review and measure Risk Management activities for effectiveness.</v>
-      </c>
-      <c r="G14" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Risk Management activities for effectiveness.</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="17">
-      <c r="A15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Security Assessment activities</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>CA.4.996</v>
-      </c>
-      <c r="E15" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>CA.4.996</v>
-      </c>
-      <c r="F15" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>CA.4.996: Review and measure Security Assessment activities for effectiveness.</v>
-      </c>
-      <c r="G15" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Security Assessment activities for effectiveness.</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="17">
-      <c r="A16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve Situational Awareness activities</v>
-      </c>
-      <c r="D16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>SA.4.996</v>
-      </c>
-      <c r="E16" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>SA.4.996</v>
-      </c>
-      <c r="F16" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>SA.4.996: Review and measure Situational Awareness activities for effectiveness.</v>
-      </c>
-      <c r="G16" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure Situational Awareness activities for effectiveness.</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="17">
-      <c r="A17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve System and Communications Protection activities</v>
-      </c>
-      <c r="D17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>SC.4.996</v>
-      </c>
-      <c r="E17" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>SC.4.996</v>
-      </c>
-      <c r="F17" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>SC.4.996: Review and measure System and Communications Protection activities for effectiveness.</v>
-      </c>
-      <c r="G17" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure System and Communications Protection activities for effectiveness.</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17">
-      <c r="A18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>CMMC v1.02 Maturity Level 4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>MC01: Improve System and Information Integrity activities</v>
-      </c>
-      <c r="D18" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>SI.4.996</v>
-      </c>
-      <c r="E18" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>SI.4.996</v>
-      </c>
-      <c r="F18" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>SI.4.996: Review and measure System and Information Integrity activities for effectiveness.</v>
-      </c>
-      <c r="G18" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Review and measure System and Information Integrity activities for effectiveness.</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E78D9C1-42B5-894D-AC78-ACB22999BE15}">
-  <dimension ref="A1:J18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="123.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="115.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="str">
         <f>"CMMC v1.02 Maturity Level 5"</f>
@@ -9592,7 +10755,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="str">
-        <f t="shared" ref="A3:A18" si="0">"CMMC v1.02 Maturity Level 5"</f>
+        <f t="shared" ref="A3:A33" si="0">"CMMC v1.02 Maturity Level 5"</f>
         <v>CMMC v1.02 Maturity Level 5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -9607,7 +10770,7 @@
         <v>AM.5.995</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f t="shared" ref="E3:E18" si="3">D3</f>
+        <f t="shared" ref="E3:E33" si="3">D3</f>
         <v>AM.5.995</v>
       </c>
       <c r="F3" s="1" t="str">
@@ -10181,7 +11344,7 @@
         <v>SI.5.995</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f>_xlfn.CONCAT(D18,": ", G18)</f>
         <v>SI.5.995: Standardize and optimize a documented approach for System and Information Integrity across all applicable organizational units.</v>
       </c>
       <c r="G18" s="1" t="str">
@@ -10198,8 +11361,444 @@
         <v>31</v>
       </c>
     </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>621</v>
+      </c>
+      <c r="E19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AC.5.024</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <f>_xlfn.CONCAT(D19,": ", G19)</f>
+        <v>AC.5.024: Identify and mitigate risk associated with unidentified wireless access points connected to the network.</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
+        <v>622</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>AU.5.055</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <f>_xlfn.CONCAT(D20,": ", G20)</f>
+        <v>AU.5.055: Identify assets not reporting audit logs and assure appropriate organizationally defined systems are logging.</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" t="s">
+        <v>623</v>
+      </c>
+      <c r="E21" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>CM.5.074</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <f>_xlfn.CONCAT(D21,": ", G21)</f>
+        <v>CM.5.074: Verify the integrity and correctness of security critical or essential software as defined by the organization (e.g., roots of trust, formal verification, or cryptographic signatures).</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" t="s">
+        <v>624</v>
+      </c>
+      <c r="E22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>IR.5.106</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <f>_xlfn.CONCAT(D22,": ", G22)</f>
+        <v>IR.5.106: In response to cyber incidents, utilize forensic data gathering across impacted systems, ensuring the secure transfer and protection of forensic data.</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" t="s">
+        <v>625</v>
+      </c>
+      <c r="E23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>IR.5.102</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f>_xlfn.CONCAT(D23,": ", G23)</f>
+        <v>IR.5.102: Use a combination of manual and automated, real-time responses to anomalous activities that match incident patterns.</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" t="s">
+        <v>626</v>
+      </c>
+      <c r="E24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>IR.5.108</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <f>_xlfn.CONCAT(D24,": ", G24)</f>
+        <v>IR.5.108: Establish and maintain a cyber incident response team that can investigate an issue physically or virtually at any location within 24 hours.</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D25" t="s">
+        <v>627</v>
+      </c>
+      <c r="E25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>IR.5.110</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <f>_xlfn.CONCAT(D25,": ", G25)</f>
+        <v>IR.5.110: Perform unannounced operational exercises to demonstrate technical and procedural responses.</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="D26" t="s">
+        <v>628</v>
+      </c>
+      <c r="E26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>RE.5.140</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <f>_xlfn.CONCAT(D26,": ", G26)</f>
+        <v>RE.5.140: Ensure information processing facilities meet organizationally defined information security continuity, redundancy, and availability requirements.</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D27" t="s">
+        <v>629</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>RM.5.152</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <f>_xlfn.CONCAT(D27,": ", G27)</f>
+        <v>RM.5.152: Utilize an exception process for non-whitelisted software that includes mitigation techniques.</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D28" t="s">
+        <v>630</v>
+      </c>
+      <c r="E28" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>RM.5.155</v>
+      </c>
+      <c r="F28" s="1" t="str">
+        <f>_xlfn.CONCAT(D28,": ", G28)</f>
+        <v>RM.5.155: Analyze the effectiveness of security solutions at least annually to address anticipated risk to the system and the organization based on current and accumulated threat intelligence.</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D29" t="s">
+        <v>566</v>
+      </c>
+      <c r="E29" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SC.5.198</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <f>_xlfn.CONCAT(D29,": ", G29)</f>
+        <v>SC.5.198: Configure monitoring systems to record packets passing through the organization's Internet network boundaries and other organizationally defined boundaries.</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D30" t="s">
+        <v>567</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SC.5.230</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <f>_xlfn.CONCAT(D30,": ", G30)</f>
+        <v>SC.5.230: Enforce port and protocol compliance.</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D31" t="s">
+        <v>631</v>
+      </c>
+      <c r="E31" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SC.5.208</v>
+      </c>
+      <c r="F31" s="1" t="str">
+        <f>_xlfn.CONCAT(D31,": ", G31)</f>
+        <v>SC.5.208: Employ organizationally defined and tailored boundary protections in addition to commercially available solutions.</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D32" t="s">
+        <v>632</v>
+      </c>
+      <c r="E32" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SI.5.222</v>
+      </c>
+      <c r="F32" s="1" t="str">
+        <f>_xlfn.CONCAT(D32,": ", G32)</f>
+        <v>SI.5.222: Analyze system behavior to detect and mitigate execution of normal system commands and scripts that indicate malicious actions.</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="17">
+      <c r="A33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>CMMC v1.02 Maturity Level 5</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D33" t="s">
+        <v>633</v>
+      </c>
+      <c r="E33" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>SI.5.223</v>
+      </c>
+      <c r="F33" s="1" t="str">
+        <f>_xlfn.CONCAT(D33,": ", G33)</f>
+        <v>SI.5.223: Monitor individuals and system components on an ongoing basis for anomalous or suspicious behavior.</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>656</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated all ML spreadsheet
</commit_message>
<xml_diff>
--- a/Control Frameworks/CMMC v1.02/CMMC v1.02 (All Maturity Levels).xlsx
+++ b/Control Frameworks/CMMC v1.02/CMMC v1.02 (All Maturity Levels).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsokol/Documents/git/simplerisk/import-content/Control Frameworks/CMMC v1.02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE72C90-D8E0-D540-B251-0CDDB3E5BE0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE1C608-1176-E84F-9075-1EB1D469DB65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20260" yWindow="460" windowWidth="30340" windowHeight="16940" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20260" yWindow="460" windowWidth="30340" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CMMC v1.02 Maturity Level 1" sheetId="3" r:id="rId1"/>
@@ -3346,7 +3346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1181B36C-6D61-4E43-8411-924D05A97DEE}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -3837,9 +3837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7062778B-DC78-BF47-BA7F-83C659A1FE69}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -6817,9 +6815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C76"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -9206,9 +9202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95FA5B7-9436-324E-80C2-1BF95F9E19C1}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C44"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -10667,7 +10661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E78D9C1-42B5-894D-AC78-ACB22999BE15}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -10774,7 +10768,7 @@
         <v>AM.5.995</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f t="shared" ref="F3:F18" si="4">_xlfn.CONCAT(D3,": ", G3)</f>
+        <f t="shared" ref="F3:F17" si="4">_xlfn.CONCAT(D3,": ", G3)</f>
         <v>AM.5.995: Standardize and optimize a documented approach for Asset Management across all applicable organizational units.</v>
       </c>
       <c r="G3" s="1" t="str">
@@ -11344,7 +11338,7 @@
         <v>SI.5.995</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>_xlfn.CONCAT(D18,": ", G18)</f>
+        <f t="shared" ref="F18:F33" si="6">_xlfn.CONCAT(D18,": ", G18)</f>
         <v>SI.5.995: Standardize and optimize a documented approach for System and Information Integrity across all applicable organizational units.</v>
       </c>
       <c r="G18" s="1" t="str">
@@ -11380,7 +11374,7 @@
         <v>AC.5.024</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>_xlfn.CONCAT(D19,": ", G19)</f>
+        <f t="shared" si="6"/>
         <v>AC.5.024: Identify and mitigate risk associated with unidentified wireless access points connected to the network.</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -11409,7 +11403,7 @@
         <v>AU.5.055</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>_xlfn.CONCAT(D20,": ", G20)</f>
+        <f t="shared" si="6"/>
         <v>AU.5.055: Identify assets not reporting audit logs and assure appropriate organizationally defined systems are logging.</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -11438,7 +11432,7 @@
         <v>CM.5.074</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>_xlfn.CONCAT(D21,": ", G21)</f>
+        <f t="shared" si="6"/>
         <v>CM.5.074: Verify the integrity and correctness of security critical or essential software as defined by the organization (e.g., roots of trust, formal verification, or cryptographic signatures).</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -11467,7 +11461,7 @@
         <v>IR.5.106</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>_xlfn.CONCAT(D22,": ", G22)</f>
+        <f t="shared" si="6"/>
         <v>IR.5.106: In response to cyber incidents, utilize forensic data gathering across impacted systems, ensuring the secure transfer and protection of forensic data.</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -11496,7 +11490,7 @@
         <v>IR.5.102</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>_xlfn.CONCAT(D23,": ", G23)</f>
+        <f t="shared" si="6"/>
         <v>IR.5.102: Use a combination of manual and automated, real-time responses to anomalous activities that match incident patterns.</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -11525,7 +11519,7 @@
         <v>IR.5.108</v>
       </c>
       <c r="F24" s="1" t="str">
-        <f>_xlfn.CONCAT(D24,": ", G24)</f>
+        <f t="shared" si="6"/>
         <v>IR.5.108: Establish and maintain a cyber incident response team that can investigate an issue physically or virtually at any location within 24 hours.</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -11554,7 +11548,7 @@
         <v>IR.5.110</v>
       </c>
       <c r="F25" s="1" t="str">
-        <f>_xlfn.CONCAT(D25,": ", G25)</f>
+        <f t="shared" si="6"/>
         <v>IR.5.110: Perform unannounced operational exercises to demonstrate technical and procedural responses.</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -11583,7 +11577,7 @@
         <v>RE.5.140</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>_xlfn.CONCAT(D26,": ", G26)</f>
+        <f t="shared" si="6"/>
         <v>RE.5.140: Ensure information processing facilities meet organizationally defined information security continuity, redundancy, and availability requirements.</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -11612,7 +11606,7 @@
         <v>RM.5.152</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f>_xlfn.CONCAT(D27,": ", G27)</f>
+        <f t="shared" si="6"/>
         <v>RM.5.152: Utilize an exception process for non-whitelisted software that includes mitigation techniques.</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -11641,7 +11635,7 @@
         <v>RM.5.155</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f>_xlfn.CONCAT(D28,": ", G28)</f>
+        <f t="shared" si="6"/>
         <v>RM.5.155: Analyze the effectiveness of security solutions at least annually to address anticipated risk to the system and the organization based on current and accumulated threat intelligence.</v>
       </c>
       <c r="G28" s="1" t="s">
@@ -11670,7 +11664,7 @@
         <v>SC.5.198</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f>_xlfn.CONCAT(D29,": ", G29)</f>
+        <f t="shared" si="6"/>
         <v>SC.5.198: Configure monitoring systems to record packets passing through the organization's Internet network boundaries and other organizationally defined boundaries.</v>
       </c>
       <c r="G29" s="1" t="s">
@@ -11699,7 +11693,7 @@
         <v>SC.5.230</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f>_xlfn.CONCAT(D30,": ", G30)</f>
+        <f t="shared" si="6"/>
         <v>SC.5.230: Enforce port and protocol compliance.</v>
       </c>
       <c r="G30" s="1" t="s">
@@ -11728,7 +11722,7 @@
         <v>SC.5.208</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>_xlfn.CONCAT(D31,": ", G31)</f>
+        <f t="shared" si="6"/>
         <v>SC.5.208: Employ organizationally defined and tailored boundary protections in addition to commercially available solutions.</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -11757,7 +11751,7 @@
         <v>SI.5.222</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>_xlfn.CONCAT(D32,": ", G32)</f>
+        <f t="shared" si="6"/>
         <v>SI.5.222: Analyze system behavior to detect and mitigate execution of normal system commands and scripts that indicate malicious actions.</v>
       </c>
       <c r="G32" s="1" t="s">
@@ -11786,7 +11780,7 @@
         <v>SI.5.223</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>_xlfn.CONCAT(D33,": ", G33)</f>
+        <f t="shared" si="6"/>
         <v>SI.5.223: Monitor individuals and system components on an ongoing basis for anomalous or suspicious behavior.</v>
       </c>
       <c r="G33" s="1" t="s">

</xml_diff>